<commit_message>
Serverside testing localhost not working
</commit_message>
<xml_diff>
--- a/schedule-server/datasheet.xlsx
+++ b/schedule-server/datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\GitHub\ScheduleAppWithWebServer\schedule-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3F2B42-537A-4414-9A73-5D3FFDB441BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2358FB9A-485C-44E5-9C03-73F5107480D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -372,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3FFB21-E2D4-4B3B-B431-08B9AE13271D}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -384,28 +384,37 @@
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>